<commit_message>
added a few drinks
</commit_message>
<xml_diff>
--- a/global_cocktails.xlsx
+++ b/global_cocktails.xlsx
@@ -311,6 +311,9 @@
     <t>Johannesburg</t>
   </si>
   <si>
+    <t>Springbokkie</t>
+  </si>
+  <si>
     <t>Saint Petersburg</t>
   </si>
   <si>
@@ -581,7 +584,7 @@
     <t>Casablanca</t>
   </si>
   <si>
-    <t>Casablanca cocktail</t>
+    <t>French 75</t>
   </si>
   <si>
     <t>Paris</t>
@@ -590,7 +593,7 @@
     <t>Sidecar</t>
   </si>
   <si>
-    <t>Kiev</t>
+    <t>Istanbul</t>
   </si>
   <si>
     <t>Dar es Salaam</t>
@@ -656,9 +659,6 @@
     <t>Khartoum</t>
   </si>
   <si>
-    <t>Pimm’s Cup</t>
-  </si>
-  <si>
     <t>Volgograd</t>
   </si>
   <si>
@@ -716,6 +716,9 @@
     <t>Cairo</t>
   </si>
   <si>
+    <t>Suffering Bastard</t>
+  </si>
+  <si>
     <t>Doha</t>
   </si>
   <si>
@@ -738,9 +741,6 @@
   </si>
   <si>
     <t>Luanda</t>
-  </si>
-  <si>
-    <t>Sofia</t>
   </si>
 </sst>
 </file>
@@ -750,7 +750,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -762,13 +762,18 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -787,8 +792,14 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -800,6 +811,28 @@
       <left style="thin">
         <color indexed="10"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="10"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="10"/>
       </right>
@@ -813,7 +846,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -822,7 +855,7 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -831,43 +864,28 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="11"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -876,28 +894,58 @@
         <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="11"/>
+      </left>
+      <right style="thin">
+        <color indexed="11"/>
+      </right>
+      <top style="thin">
+        <color indexed="11"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -907,44 +955,50 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -964,8 +1018,10 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
     </indexedColors>
@@ -984,10 +1040,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -1164,11 +1220,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:schemeClr val="accent1"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1177,7 +1236,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1192,12 +1251,12 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -1454,10 +1513,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1748,7 +1807,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -2029,31 +2088,28 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:BC23"/>
+  <dimension ref="A1:BC23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.2969" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.2266" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.63281" style="1" customWidth="1"/>
-    <col min="4" max="4" width="8.22656" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.8438" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.10156" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.0469" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.3516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1719" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.67188" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.17188" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.8516" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.17188" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.5" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.5234" style="1" customWidth="1"/>
-    <col min="10" max="10" width="10.4062" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6328" style="1" customWidth="1"/>
-    <col min="12" max="12" width="11.0625" style="1" customWidth="1"/>
-    <col min="13" max="19" width="8.45312" style="1" customWidth="1"/>
-    <col min="20" max="21" width="9.04688" style="1" customWidth="1"/>
-    <col min="22" max="22" width="9.60156" style="1" customWidth="1"/>
-    <col min="23" max="23" width="9.74219" style="1" customWidth="1"/>
-    <col min="24" max="55" width="9.76562" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.5" style="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="10.6719" style="1" customWidth="1"/>
+    <col min="12" max="12" width="11" style="1" customWidth="1"/>
+    <col min="13" max="19" width="8.5" style="1" customWidth="1"/>
+    <col min="20" max="21" width="9" style="1" customWidth="1"/>
+    <col min="22" max="22" width="9.67188" style="1" customWidth="1"/>
+    <col min="23" max="55" width="9.85156" style="1" customWidth="1"/>
     <col min="56" max="256" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2061,1804 +2117,1804 @@
       <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-      <c r="AA1" s="2"/>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="2"/>
-      <c r="AD1" s="2"/>
-      <c r="AE1" s="2"/>
-      <c r="AF1" s="2"/>
-      <c r="AG1" s="2"/>
-      <c r="AH1" s="2"/>
-      <c r="AI1" s="2"/>
-      <c r="AJ1" s="2"/>
-      <c r="AK1" s="2"/>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2"/>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2"/>
-      <c r="AR1" s="2"/>
-      <c r="AS1" s="2"/>
-      <c r="AT1" s="2"/>
-      <c r="AU1" s="2"/>
-      <c r="AV1" s="2"/>
-      <c r="AW1" s="2"/>
-      <c r="AX1" s="2"/>
-      <c r="AY1" s="2"/>
-      <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+      <c r="U1" s="3"/>
+      <c r="V1" s="3"/>
+      <c r="W1" s="3"/>
+      <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="3"/>
+      <c r="AB1" s="3"/>
+      <c r="AC1" s="3"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
+      <c r="AF1" s="3"/>
+      <c r="AG1" s="3"/>
+      <c r="AH1" s="3"/>
+      <c r="AI1" s="3"/>
+      <c r="AJ1" s="3"/>
+      <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
+      <c r="AM1" s="3"/>
+      <c r="AN1" s="3"/>
+      <c r="AO1" s="3"/>
+      <c r="AP1" s="3"/>
+      <c r="AQ1" s="3"/>
+      <c r="AR1" s="3"/>
+      <c r="AS1" s="3"/>
+      <c r="AT1" s="3"/>
+      <c r="AU1" s="3"/>
+      <c r="AV1" s="3"/>
+      <c r="AW1" s="3"/>
+      <c r="AX1" s="3"/>
+      <c r="AY1" s="3"/>
+      <c r="AZ1" s="3"/>
+      <c r="BA1" s="3"/>
+      <c r="BB1" s="3"/>
+      <c r="BC1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
-      <c r="AJ2" s="3"/>
-      <c r="AK2" s="3"/>
-      <c r="AL2" s="3"/>
-      <c r="AM2" s="3"/>
-      <c r="AN2" s="3"/>
-      <c r="AO2" s="3"/>
-      <c r="AP2" s="3"/>
-      <c r="AQ2" s="3"/>
-      <c r="AR2" s="3"/>
-      <c r="AS2" s="3"/>
-      <c r="AT2" s="3"/>
-      <c r="AU2" s="3"/>
-      <c r="AV2" s="3"/>
-      <c r="AW2" s="3"/>
-      <c r="AX2" s="3"/>
-      <c r="AY2" s="3"/>
-      <c r="AZ2" s="3"/>
-      <c r="BA2" s="3"/>
-      <c r="BB2" s="3"/>
-      <c r="BC2" s="3"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
+      <c r="W2" s="5"/>
+      <c r="X2" s="5"/>
+      <c r="Y2" s="5"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5"/>
+      <c r="AC2" s="5"/>
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
+      <c r="AH2" s="5"/>
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AN2" s="5"/>
+      <c r="AO2" s="5"/>
+      <c r="AP2" s="5"/>
+      <c r="AQ2" s="5"/>
+      <c r="AR2" s="5"/>
+      <c r="AS2" s="5"/>
+      <c r="AT2" s="5"/>
+      <c r="AU2" s="5"/>
+      <c r="AV2" s="5"/>
+      <c r="AW2" s="5"/>
+      <c r="AX2" s="5"/>
+      <c r="AY2" s="5"/>
+      <c r="AZ2" s="5"/>
+      <c r="BA2" s="5"/>
+      <c r="BB2" s="5"/>
+      <c r="BC2" s="5"/>
     </row>
     <row r="3" ht="44.25" customHeight="1">
-      <c r="A3" s="4"/>
-      <c r="B3" t="s" s="5">
+      <c r="A3" s="6"/>
+      <c r="B3" t="s" s="7">
         <v>1</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="6"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
-      <c r="AP3" s="6"/>
-      <c r="AQ3" s="6"/>
-      <c r="AR3" s="6"/>
-      <c r="AS3" s="6"/>
-      <c r="AT3" s="6"/>
-      <c r="AU3" s="6"/>
-      <c r="AV3" s="6"/>
-      <c r="AW3" s="6"/>
-      <c r="AX3" t="s" s="7">
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8"/>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8"/>
+      <c r="AG3" s="8"/>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="8"/>
+      <c r="AJ3" s="8"/>
+      <c r="AK3" s="8"/>
+      <c r="AL3" s="8"/>
+      <c r="AM3" s="8"/>
+      <c r="AN3" s="8"/>
+      <c r="AO3" s="8"/>
+      <c r="AP3" s="8"/>
+      <c r="AQ3" s="8"/>
+      <c r="AR3" s="8"/>
+      <c r="AS3" s="8"/>
+      <c r="AT3" s="8"/>
+      <c r="AU3" s="8"/>
+      <c r="AV3" s="8"/>
+      <c r="AW3" s="8"/>
+      <c r="AX3" t="s" s="9">
         <v>2</v>
       </c>
-      <c r="AY3" s="6"/>
-      <c r="AZ3" t="s" s="7">
+      <c r="AY3" s="8"/>
+      <c r="AZ3" t="s" s="9">
         <v>3</v>
       </c>
-      <c r="BA3" s="6"/>
-      <c r="BB3" s="6"/>
-      <c r="BC3" s="6"/>
+      <c r="BA3" s="8"/>
+      <c r="BB3" s="8"/>
+      <c r="BC3" s="8"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="8"/>
-      <c r="B4" t="s" s="9">
+      <c r="A4" s="10"/>
+      <c r="B4" t="s" s="11">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" t="s" s="11">
+      <c r="C4" s="12"/>
+      <c r="D4" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" t="s" s="11">
+      <c r="E4" s="12"/>
+      <c r="F4" t="s" s="13">
         <v>6</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" t="s" s="11">
+      <c r="G4" s="12"/>
+      <c r="H4" t="s" s="13">
         <v>7</v>
       </c>
-      <c r="I4" s="10"/>
-      <c r="J4" t="s" s="11">
+      <c r="I4" s="12"/>
+      <c r="J4" t="s" s="13">
         <v>8</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" t="s" s="11">
+      <c r="K4" s="12"/>
+      <c r="L4" t="s" s="13">
         <v>9</v>
       </c>
-      <c r="M4" s="10"/>
-      <c r="N4" t="s" s="11">
+      <c r="M4" s="12"/>
+      <c r="N4" t="s" s="13">
         <v>10</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" t="s" s="11">
+      <c r="O4" s="12"/>
+      <c r="P4" t="s" s="13">
         <v>11</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" t="s" s="11">
+      <c r="Q4" s="12"/>
+      <c r="R4" t="s" s="13">
         <v>12</v>
       </c>
-      <c r="S4" s="10"/>
-      <c r="T4" t="s" s="11">
+      <c r="S4" s="12"/>
+      <c r="T4" t="s" s="13">
         <v>13</v>
       </c>
-      <c r="U4" s="10"/>
-      <c r="V4" t="s" s="11">
+      <c r="U4" s="12"/>
+      <c r="V4" t="s" s="13">
         <v>14</v>
       </c>
-      <c r="W4" s="10"/>
-      <c r="X4" t="s" s="11">
+      <c r="W4" s="12"/>
+      <c r="X4" t="s" s="13">
         <v>15</v>
       </c>
-      <c r="Y4" s="10"/>
-      <c r="Z4" t="s" s="11">
+      <c r="Y4" s="12"/>
+      <c r="Z4" t="s" s="13">
         <v>16</v>
       </c>
-      <c r="AA4" s="10"/>
-      <c r="AB4" t="s" s="11">
+      <c r="AA4" s="12"/>
+      <c r="AB4" t="s" s="13">
         <v>17</v>
       </c>
-      <c r="AC4" s="10"/>
-      <c r="AD4" t="s" s="11">
+      <c r="AC4" s="12"/>
+      <c r="AD4" t="s" s="13">
         <v>18</v>
       </c>
-      <c r="AE4" s="10"/>
-      <c r="AF4" t="s" s="11">
+      <c r="AE4" s="12"/>
+      <c r="AF4" t="s" s="13">
         <v>19</v>
       </c>
-      <c r="AG4" s="10"/>
-      <c r="AH4" t="s" s="11">
+      <c r="AG4" s="12"/>
+      <c r="AH4" t="s" s="13">
         <v>20</v>
       </c>
-      <c r="AI4" s="10"/>
-      <c r="AJ4" t="s" s="11">
+      <c r="AI4" s="12"/>
+      <c r="AJ4" t="s" s="13">
         <v>21</v>
       </c>
-      <c r="AK4" s="10"/>
-      <c r="AL4" t="s" s="11">
+      <c r="AK4" s="12"/>
+      <c r="AL4" t="s" s="13">
         <v>22</v>
       </c>
-      <c r="AM4" s="10"/>
-      <c r="AN4" t="s" s="11">
+      <c r="AM4" s="12"/>
+      <c r="AN4" t="s" s="13">
         <v>23</v>
       </c>
-      <c r="AO4" s="10"/>
-      <c r="AP4" t="s" s="11">
+      <c r="AO4" s="12"/>
+      <c r="AP4" t="s" s="13">
         <v>24</v>
       </c>
-      <c r="AQ4" s="10"/>
-      <c r="AR4" t="s" s="11">
+      <c r="AQ4" s="12"/>
+      <c r="AR4" t="s" s="13">
         <v>25</v>
       </c>
-      <c r="AS4" s="10"/>
-      <c r="AT4" t="s" s="11">
+      <c r="AS4" s="12"/>
+      <c r="AT4" t="s" s="13">
         <v>26</v>
       </c>
-      <c r="AU4" s="10"/>
-      <c r="AV4" t="s" s="11">
+      <c r="AU4" s="12"/>
+      <c r="AV4" t="s" s="13">
         <v>27</v>
       </c>
-      <c r="AW4" s="10"/>
-      <c r="AX4" t="s" s="11">
+      <c r="AW4" s="12"/>
+      <c r="AX4" t="s" s="13">
         <v>28</v>
       </c>
-      <c r="AY4" s="10"/>
-      <c r="AZ4" t="s" s="11">
+      <c r="AY4" s="12"/>
+      <c r="AZ4" t="s" s="13">
         <v>29</v>
       </c>
-      <c r="BA4" s="10"/>
-      <c r="BB4" s="10"/>
-      <c r="BC4" s="10"/>
+      <c r="BA4" s="12"/>
+      <c r="BB4" s="12"/>
+      <c r="BC4" s="12"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" t="s" s="9">
+      <c r="A5" s="10"/>
+      <c r="B5" t="s" s="11">
         <v>30</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" t="s" s="13">
         <v>31</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
-      <c r="Q5" s="10"/>
-      <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
-      <c r="T5" s="10"/>
-      <c r="U5" s="10"/>
-      <c r="V5" s="10"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="10"/>
-      <c r="Z5" s="10"/>
-      <c r="AA5" s="10"/>
-      <c r="AB5" s="10"/>
-      <c r="AC5" s="10"/>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="10"/>
-      <c r="AF5" s="10"/>
-      <c r="AG5" s="10"/>
-      <c r="AH5" s="10"/>
-      <c r="AI5" s="10"/>
-      <c r="AJ5" s="10"/>
-      <c r="AK5" s="10"/>
-      <c r="AL5" s="10"/>
-      <c r="AM5" s="10"/>
-      <c r="AN5" s="10"/>
-      <c r="AO5" s="10"/>
-      <c r="AP5" s="10"/>
-      <c r="AQ5" s="10"/>
-      <c r="AR5" s="10"/>
-      <c r="AS5" s="10"/>
-      <c r="AT5" s="10"/>
-      <c r="AU5" s="10"/>
-      <c r="AV5" s="10"/>
-      <c r="AW5" s="10"/>
-      <c r="AX5" s="10"/>
-      <c r="AY5" s="10"/>
-      <c r="AZ5" s="10"/>
-      <c r="BA5" s="10"/>
-      <c r="BB5" s="10"/>
-      <c r="BC5" s="10"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="12"/>
+      <c r="AJ5" s="12"/>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12"/>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12"/>
+      <c r="AO5" s="12"/>
+      <c r="AP5" s="12"/>
+      <c r="AQ5" s="12"/>
+      <c r="AR5" s="12"/>
+      <c r="AS5" s="12"/>
+      <c r="AT5" s="12"/>
+      <c r="AU5" s="12"/>
+      <c r="AV5" s="12"/>
+      <c r="AW5" s="12"/>
+      <c r="AX5" s="12"/>
+      <c r="AY5" s="12"/>
+      <c r="AZ5" s="12"/>
+      <c r="BA5" s="12"/>
+      <c r="BB5" s="12"/>
+      <c r="BC5" s="12"/>
     </row>
     <row r="6" ht="44.05" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" t="s" s="9">
+      <c r="A6" s="10"/>
+      <c r="B6" t="s" s="11">
         <v>32</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" t="s" s="13">
         <v>33</v>
       </c>
-      <c r="D6" t="s" s="11">
+      <c r="D6" t="s" s="13">
         <v>34</v>
       </c>
-      <c r="E6" t="s" s="11">
+      <c r="E6" t="s" s="13">
         <v>35</v>
       </c>
-      <c r="F6" t="s" s="11">
+      <c r="F6" t="s" s="13">
         <v>36</v>
       </c>
-      <c r="G6" t="s" s="11">
+      <c r="G6" t="s" s="13">
         <v>37</v>
       </c>
-      <c r="H6" t="s" s="11">
+      <c r="H6" t="s" s="13">
         <v>38</v>
       </c>
-      <c r="I6" t="s" s="11">
+      <c r="I6" t="s" s="13">
         <v>39</v>
       </c>
-      <c r="J6" t="s" s="11">
+      <c r="J6" t="s" s="13">
         <v>40</v>
       </c>
-      <c r="K6" t="s" s="11">
+      <c r="K6" t="s" s="13">
         <v>41</v>
       </c>
-      <c r="L6" t="s" s="11">
+      <c r="L6" t="s" s="13">
         <v>42</v>
       </c>
-      <c r="M6" s="10"/>
-      <c r="N6" t="s" s="11">
+      <c r="M6" s="12"/>
+      <c r="N6" t="s" s="13">
         <v>43</v>
       </c>
-      <c r="O6" t="s" s="11">
+      <c r="O6" t="s" s="13">
         <v>44</v>
       </c>
-      <c r="P6" t="s" s="11">
+      <c r="P6" t="s" s="13">
         <v>45</v>
       </c>
-      <c r="Q6" t="s" s="11">
+      <c r="Q6" t="s" s="13">
         <v>46</v>
       </c>
-      <c r="R6" t="s" s="11">
+      <c r="R6" t="s" s="13">
         <v>47</v>
       </c>
-      <c r="S6" t="s" s="11">
+      <c r="S6" t="s" s="13">
         <v>48</v>
       </c>
-      <c r="T6" t="s" s="11">
+      <c r="T6" t="s" s="13">
         <v>49</v>
       </c>
-      <c r="U6" t="s" s="11">
+      <c r="U6" t="s" s="13">
         <v>50</v>
       </c>
-      <c r="V6" t="s" s="11">
+      <c r="V6" t="s" s="13">
         <v>51</v>
       </c>
-      <c r="W6" t="s" s="11">
+      <c r="W6" t="s" s="13">
         <v>52</v>
       </c>
-      <c r="X6" t="s" s="11">
+      <c r="X6" t="s" s="13">
         <v>53</v>
       </c>
-      <c r="Y6" t="s" s="11">
+      <c r="Y6" t="s" s="13">
         <v>54</v>
       </c>
-      <c r="Z6" t="s" s="11">
+      <c r="Z6" t="s" s="13">
         <v>55</v>
       </c>
-      <c r="AA6" t="s" s="11">
+      <c r="AA6" t="s" s="13">
         <v>56</v>
       </c>
-      <c r="AB6" t="s" s="11">
+      <c r="AB6" t="s" s="13">
         <v>57</v>
       </c>
-      <c r="AC6" t="s" s="11">
+      <c r="AC6" t="s" s="13">
         <v>58</v>
       </c>
-      <c r="AD6" t="s" s="11">
+      <c r="AD6" t="s" s="13">
         <v>59</v>
       </c>
-      <c r="AE6" t="s" s="11">
+      <c r="AE6" t="s" s="13">
         <v>60</v>
       </c>
-      <c r="AF6" t="s" s="11">
+      <c r="AF6" t="s" s="13">
         <v>61</v>
       </c>
-      <c r="AG6" s="10"/>
-      <c r="AH6" t="s" s="11">
+      <c r="AG6" s="12"/>
+      <c r="AH6" t="s" s="13">
         <v>62</v>
       </c>
-      <c r="AI6" t="s" s="11">
+      <c r="AI6" t="s" s="13">
         <v>63</v>
       </c>
-      <c r="AJ6" t="s" s="11">
+      <c r="AJ6" t="s" s="13">
         <v>64</v>
       </c>
-      <c r="AK6" t="s" s="11">
+      <c r="AK6" t="s" s="13">
         <v>65</v>
       </c>
-      <c r="AL6" t="s" s="11">
+      <c r="AL6" t="s" s="13">
         <v>66</v>
       </c>
-      <c r="AM6" t="s" s="11">
+      <c r="AM6" t="s" s="13">
         <v>67</v>
       </c>
-      <c r="AN6" t="s" s="11">
+      <c r="AN6" t="s" s="13">
         <v>68</v>
       </c>
-      <c r="AO6" t="s" s="11">
+      <c r="AO6" t="s" s="13">
         <v>69</v>
       </c>
-      <c r="AP6" t="s" s="11">
+      <c r="AP6" t="s" s="13">
         <v>70</v>
       </c>
-      <c r="AQ6" t="s" s="11">
+      <c r="AQ6" t="s" s="13">
         <v>71</v>
       </c>
-      <c r="AR6" t="s" s="11">
+      <c r="AR6" t="s" s="13">
         <v>72</v>
       </c>
-      <c r="AS6" t="s" s="11">
+      <c r="AS6" t="s" s="13">
         <v>73</v>
       </c>
-      <c r="AT6" t="s" s="11">
+      <c r="AT6" t="s" s="13">
         <v>74</v>
       </c>
-      <c r="AU6" s="10"/>
-      <c r="AV6" t="s" s="11">
+      <c r="AU6" s="12"/>
+      <c r="AV6" t="s" s="13">
         <v>75</v>
       </c>
-      <c r="AW6" t="s" s="11">
+      <c r="AW6" t="s" s="13">
         <v>76</v>
       </c>
-      <c r="AX6" t="s" s="11">
+      <c r="AX6" t="s" s="13">
         <v>77</v>
       </c>
-      <c r="AY6" s="10"/>
-      <c r="AZ6" t="s" s="11">
+      <c r="AY6" s="12"/>
+      <c r="AZ6" t="s" s="13">
         <v>78</v>
       </c>
-      <c r="BA6" s="10"/>
-      <c r="BB6" s="10"/>
-      <c r="BC6" s="10"/>
+      <c r="BA6" s="12"/>
+      <c r="BB6" s="12"/>
+      <c r="BC6" s="12"/>
     </row>
     <row r="7" ht="44.05" customHeight="1">
-      <c r="A7" s="8"/>
-      <c r="B7" t="s" s="9">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="11">
         <v>79</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" t="s" s="11">
+      <c r="C7" s="12"/>
+      <c r="D7" t="s" s="13">
         <v>80</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" t="s" s="11">
+      <c r="E7" s="12"/>
+      <c r="F7" t="s" s="13">
         <v>81</v>
       </c>
-      <c r="G7" t="s" s="11">
+      <c r="G7" t="s" s="13">
         <v>82</v>
       </c>
-      <c r="H7" t="s" s="11">
+      <c r="H7" t="s" s="13">
         <v>83</v>
       </c>
-      <c r="I7" t="s" s="11">
+      <c r="I7" t="s" s="13">
         <v>84</v>
       </c>
-      <c r="J7" t="s" s="11">
+      <c r="J7" t="s" s="13">
         <v>85</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" t="s" s="11">
+      <c r="K7" s="12"/>
+      <c r="L7" t="s" s="13">
         <v>86</v>
       </c>
-      <c r="M7" t="s" s="11">
+      <c r="M7" t="s" s="13">
         <v>87</v>
       </c>
-      <c r="N7" t="s" s="11">
+      <c r="N7" t="s" s="13">
         <v>88</v>
       </c>
-      <c r="O7" s="10"/>
-      <c r="P7" t="s" s="11">
+      <c r="O7" s="12"/>
+      <c r="P7" t="s" s="13">
         <v>89</v>
       </c>
-      <c r="Q7" t="s" s="11">
+      <c r="Q7" t="s" s="13">
         <v>90</v>
       </c>
-      <c r="R7" t="s" s="11">
+      <c r="R7" t="s" s="13">
         <v>91</v>
       </c>
-      <c r="S7" t="s" s="11">
+      <c r="S7" t="s" s="13">
         <v>50</v>
       </c>
-      <c r="T7" s="10"/>
-      <c r="U7" s="10"/>
-      <c r="V7" t="s" s="11">
+      <c r="T7" s="12"/>
+      <c r="U7" s="12"/>
+      <c r="V7" t="s" s="13">
         <v>92</v>
       </c>
-      <c r="W7" t="s" s="11">
+      <c r="W7" t="s" s="13">
         <v>93</v>
       </c>
-      <c r="X7" t="s" s="11">
+      <c r="X7" t="s" s="13">
         <v>94</v>
       </c>
-      <c r="Y7" t="s" s="11">
+      <c r="Y7" t="s" s="13">
         <v>95</v>
       </c>
-      <c r="Z7" t="s" s="11">
+      <c r="Z7" t="s" s="13">
         <v>96</v>
       </c>
-      <c r="AA7" t="s" s="11">
+      <c r="AA7" t="s" s="13">
         <v>97</v>
       </c>
-      <c r="AB7" t="s" s="11">
+      <c r="AB7" t="s" s="13">
         <v>98</v>
       </c>
-      <c r="AC7" s="10"/>
-      <c r="AD7" t="s" s="11">
+      <c r="AC7" t="s" s="13">
         <v>99</v>
       </c>
-      <c r="AE7" t="s" s="11">
+      <c r="AD7" t="s" s="13">
         <v>100</v>
       </c>
-      <c r="AF7" t="s" s="11">
+      <c r="AE7" t="s" s="13">
         <v>101</v>
       </c>
-      <c r="AG7" s="10"/>
-      <c r="AH7" t="s" s="11">
+      <c r="AF7" t="s" s="13">
         <v>102</v>
       </c>
-      <c r="AI7" s="10"/>
-      <c r="AJ7" t="s" s="11">
+      <c r="AG7" s="12"/>
+      <c r="AH7" t="s" s="13">
         <v>103</v>
       </c>
-      <c r="AK7" t="s" s="11">
+      <c r="AI7" s="12"/>
+      <c r="AJ7" t="s" s="13">
         <v>104</v>
       </c>
-      <c r="AL7" t="s" s="11">
+      <c r="AK7" t="s" s="13">
         <v>105</v>
       </c>
-      <c r="AM7" t="s" s="11">
+      <c r="AL7" t="s" s="13">
         <v>106</v>
       </c>
-      <c r="AN7" t="s" s="11">
+      <c r="AM7" t="s" s="13">
         <v>107</v>
       </c>
-      <c r="AO7" t="s" s="11">
+      <c r="AN7" t="s" s="13">
         <v>108</v>
       </c>
-      <c r="AP7" t="s" s="11">
+      <c r="AO7" t="s" s="13">
         <v>109</v>
       </c>
-      <c r="AQ7" t="s" s="11">
+      <c r="AP7" t="s" s="13">
         <v>110</v>
       </c>
-      <c r="AR7" t="s" s="11">
+      <c r="AQ7" t="s" s="13">
         <v>111</v>
       </c>
-      <c r="AS7" t="s" s="11">
+      <c r="AR7" t="s" s="13">
         <v>112</v>
       </c>
-      <c r="AT7" t="s" s="11">
+      <c r="AS7" t="s" s="13">
         <v>113</v>
       </c>
-      <c r="AU7" s="10"/>
-      <c r="AV7" t="s" s="11">
+      <c r="AT7" t="s" s="13">
         <v>114</v>
       </c>
-      <c r="AW7" t="s" s="11">
+      <c r="AU7" s="12"/>
+      <c r="AV7" t="s" s="13">
         <v>115</v>
       </c>
-      <c r="AX7" t="s" s="11">
+      <c r="AW7" t="s" s="13">
         <v>116</v>
       </c>
-      <c r="AY7" s="10"/>
-      <c r="AZ7" s="10"/>
-      <c r="BA7" s="10"/>
-      <c r="BB7" s="10"/>
-      <c r="BC7" s="10"/>
+      <c r="AX7" t="s" s="13">
+        <v>117</v>
+      </c>
+      <c r="AY7" s="12"/>
+      <c r="AZ7" s="12"/>
+      <c r="BA7" s="12"/>
+      <c r="BB7" s="12"/>
+      <c r="BC7" s="12"/>
     </row>
     <row r="8" ht="44.05" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="10"/>
-      <c r="D8" t="s" s="11">
-        <v>117</v>
-      </c>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" t="s" s="11">
+      <c r="A8" s="10"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="12"/>
+      <c r="D8" t="s" s="13">
         <v>118</v>
       </c>
-      <c r="I8" t="s" s="11">
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" t="s" s="13">
         <v>119</v>
       </c>
-      <c r="J8" t="s" s="11">
+      <c r="I8" t="s" s="13">
         <v>120</v>
       </c>
-      <c r="K8" t="s" s="11">
+      <c r="J8" t="s" s="13">
         <v>121</v>
       </c>
-      <c r="L8" t="s" s="11">
+      <c r="K8" t="s" s="13">
         <v>122</v>
       </c>
-      <c r="M8" t="s" s="11">
+      <c r="L8" t="s" s="13">
         <v>123</v>
       </c>
-      <c r="N8" t="s" s="11">
+      <c r="M8" t="s" s="13">
         <v>124</v>
       </c>
-      <c r="O8" t="s" s="11">
+      <c r="N8" t="s" s="13">
         <v>125</v>
       </c>
-      <c r="P8" t="s" s="11">
+      <c r="O8" t="s" s="13">
         <v>126</v>
       </c>
-      <c r="Q8" s="10"/>
-      <c r="R8" t="s" s="11">
+      <c r="P8" t="s" s="13">
         <v>127</v>
       </c>
-      <c r="S8" t="s" s="11">
+      <c r="Q8" s="12"/>
+      <c r="R8" t="s" s="13">
         <v>128</v>
       </c>
-      <c r="T8" s="10"/>
-      <c r="U8" s="10"/>
-      <c r="V8" s="10"/>
-      <c r="W8" s="10"/>
-      <c r="X8" t="s" s="11">
+      <c r="S8" t="s" s="13">
         <v>129</v>
       </c>
-      <c r="Y8" s="10"/>
-      <c r="Z8" t="s" s="11">
+      <c r="T8" s="12"/>
+      <c r="U8" s="12"/>
+      <c r="V8" s="12"/>
+      <c r="W8" s="12"/>
+      <c r="X8" t="s" s="13">
         <v>130</v>
       </c>
-      <c r="AA8" s="10"/>
-      <c r="AB8" t="s" s="11">
+      <c r="Y8" s="12"/>
+      <c r="Z8" t="s" s="13">
         <v>131</v>
       </c>
-      <c r="AC8" t="s" s="11">
+      <c r="AA8" s="12"/>
+      <c r="AB8" t="s" s="13">
         <v>132</v>
       </c>
-      <c r="AD8" t="s" s="11">
+      <c r="AC8" t="s" s="13">
         <v>133</v>
       </c>
-      <c r="AE8" t="s" s="11">
+      <c r="AD8" t="s" s="13">
+        <v>134</v>
+      </c>
+      <c r="AE8" t="s" s="13">
         <v>97</v>
       </c>
-      <c r="AF8" t="s" s="11">
-        <v>134</v>
-      </c>
-      <c r="AG8" t="s" s="11">
+      <c r="AF8" t="s" s="13">
         <v>135</v>
       </c>
-      <c r="AH8" t="s" s="11">
+      <c r="AG8" t="s" s="13">
         <v>136</v>
       </c>
-      <c r="AI8" t="s" s="11">
+      <c r="AH8" t="s" s="13">
         <v>137</v>
       </c>
-      <c r="AJ8" t="s" s="11">
+      <c r="AI8" t="s" s="13">
         <v>138</v>
       </c>
-      <c r="AK8" t="s" s="11">
+      <c r="AJ8" t="s" s="13">
         <v>139</v>
       </c>
-      <c r="AL8" t="s" s="11">
+      <c r="AK8" t="s" s="13">
         <v>140</v>
       </c>
-      <c r="AM8" s="10"/>
-      <c r="AN8" t="s" s="11">
+      <c r="AL8" t="s" s="13">
         <v>141</v>
       </c>
-      <c r="AO8" s="10"/>
-      <c r="AP8" t="s" s="11">
+      <c r="AM8" s="12"/>
+      <c r="AN8" t="s" s="13">
         <v>142</v>
       </c>
-      <c r="AQ8" t="s" s="11">
+      <c r="AO8" s="12"/>
+      <c r="AP8" t="s" s="13">
         <v>143</v>
       </c>
-      <c r="AR8" t="s" s="11">
+      <c r="AQ8" t="s" s="13">
         <v>144</v>
       </c>
-      <c r="AS8" t="s" s="11">
+      <c r="AR8" t="s" s="13">
         <v>145</v>
       </c>
-      <c r="AT8" t="s" s="11">
+      <c r="AS8" t="s" s="13">
         <v>146</v>
       </c>
-      <c r="AU8" t="s" s="11">
+      <c r="AT8" t="s" s="13">
         <v>147</v>
       </c>
-      <c r="AV8" t="s" s="11">
+      <c r="AU8" t="s" s="13">
         <v>148</v>
       </c>
-      <c r="AW8" s="10"/>
-      <c r="AX8" s="10"/>
-      <c r="AY8" s="10"/>
-      <c r="AZ8" s="10"/>
-      <c r="BA8" s="10"/>
-      <c r="BB8" s="10"/>
-      <c r="BC8" s="10"/>
+      <c r="AV8" t="s" s="13">
+        <v>149</v>
+      </c>
+      <c r="AW8" s="12"/>
+      <c r="AX8" s="12"/>
+      <c r="AY8" s="12"/>
+      <c r="AZ8" s="12"/>
+      <c r="BA8" s="12"/>
+      <c r="BB8" s="12"/>
+      <c r="BC8" s="12"/>
     </row>
     <row r="9" ht="32.05" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="10"/>
-      <c r="D9" t="s" s="11">
-        <v>149</v>
-      </c>
-      <c r="E9" t="s" s="11">
+      <c r="A9" s="10"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="12"/>
+      <c r="D9" t="s" s="13">
         <v>150</v>
       </c>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" t="s" s="11">
+      <c r="E9" t="s" s="13">
         <v>151</v>
       </c>
-      <c r="I9" s="10"/>
-      <c r="J9" t="s" s="11">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" t="s" s="13">
         <v>152</v>
       </c>
-      <c r="K9" t="s" s="11">
+      <c r="I9" s="12"/>
+      <c r="J9" t="s" s="13">
         <v>153</v>
       </c>
-      <c r="L9" t="s" s="11">
+      <c r="K9" t="s" s="13">
         <v>154</v>
       </c>
-      <c r="M9" s="10"/>
-      <c r="N9" t="s" s="11">
+      <c r="L9" t="s" s="13">
         <v>155</v>
       </c>
-      <c r="O9" t="s" s="11">
+      <c r="M9" s="12"/>
+      <c r="N9" t="s" s="13">
         <v>156</v>
       </c>
-      <c r="P9" t="s" s="11">
+      <c r="O9" t="s" s="13">
         <v>157</v>
       </c>
-      <c r="Q9" s="10"/>
-      <c r="R9" t="s" s="11">
+      <c r="P9" t="s" s="13">
         <v>158</v>
       </c>
-      <c r="S9" t="s" s="11">
+      <c r="Q9" s="12"/>
+      <c r="R9" t="s" s="13">
         <v>159</v>
       </c>
-      <c r="T9" s="10"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" t="s" s="11">
+      <c r="S9" t="s" s="13">
         <v>160</v>
       </c>
-      <c r="Y9" t="s" s="11">
+      <c r="T9" s="12"/>
+      <c r="U9" s="12"/>
+      <c r="V9" s="12"/>
+      <c r="W9" s="12"/>
+      <c r="X9" t="s" s="13">
         <v>161</v>
       </c>
-      <c r="Z9" t="s" s="11">
+      <c r="Y9" t="s" s="13">
         <v>162</v>
       </c>
-      <c r="AA9" t="s" s="11">
+      <c r="Z9" t="s" s="13">
         <v>163</v>
       </c>
-      <c r="AB9" t="s" s="11">
+      <c r="AA9" t="s" s="13">
         <v>164</v>
       </c>
-      <c r="AC9" t="s" s="11">
+      <c r="AB9" t="s" s="13">
         <v>165</v>
       </c>
-      <c r="AD9" t="s" s="11">
+      <c r="AC9" t="s" s="13">
         <v>166</v>
       </c>
-      <c r="AE9" t="s" s="11">
+      <c r="AD9" t="s" s="13">
         <v>167</v>
       </c>
-      <c r="AF9" t="s" s="11">
+      <c r="AE9" t="s" s="13">
         <v>168</v>
       </c>
-      <c r="AG9" t="s" s="11">
+      <c r="AF9" t="s" s="13">
         <v>169</v>
       </c>
-      <c r="AH9" t="s" s="11">
+      <c r="AG9" t="s" s="13">
         <v>170</v>
       </c>
-      <c r="AI9" t="s" s="11">
+      <c r="AH9" t="s" s="13">
         <v>171</v>
       </c>
-      <c r="AJ9" t="s" s="11">
+      <c r="AI9" t="s" s="13">
         <v>172</v>
       </c>
-      <c r="AK9" s="10"/>
-      <c r="AL9" t="s" s="11">
+      <c r="AJ9" t="s" s="13">
         <v>173</v>
       </c>
-      <c r="AM9" t="s" s="11">
+      <c r="AK9" s="12"/>
+      <c r="AL9" t="s" s="13">
         <v>174</v>
       </c>
-      <c r="AN9" t="s" s="11">
+      <c r="AM9" t="s" s="13">
         <v>175</v>
       </c>
-      <c r="AO9" s="10"/>
-      <c r="AP9" t="s" s="11">
+      <c r="AN9" t="s" s="13">
         <v>176</v>
       </c>
-      <c r="AQ9" s="10"/>
-      <c r="AR9" t="s" s="11">
+      <c r="AO9" s="12"/>
+      <c r="AP9" t="s" s="13">
         <v>177</v>
       </c>
-      <c r="AS9" s="10"/>
-      <c r="AT9" t="s" s="11">
+      <c r="AQ9" s="12"/>
+      <c r="AR9" t="s" s="13">
         <v>178</v>
       </c>
-      <c r="AU9" t="s" s="11">
+      <c r="AS9" s="12"/>
+      <c r="AT9" t="s" s="13">
         <v>179</v>
       </c>
-      <c r="AV9" t="s" s="11">
+      <c r="AU9" t="s" s="13">
         <v>180</v>
       </c>
-      <c r="AW9" s="10"/>
-      <c r="AX9" s="10"/>
-      <c r="AY9" s="10"/>
-      <c r="AZ9" s="10"/>
-      <c r="BA9" s="10"/>
-      <c r="BB9" s="10"/>
-      <c r="BC9" s="10"/>
+      <c r="AV9" t="s" s="13">
+        <v>181</v>
+      </c>
+      <c r="AW9" s="12"/>
+      <c r="AX9" s="12"/>
+      <c r="AY9" s="12"/>
+      <c r="AZ9" s="12"/>
+      <c r="BA9" s="12"/>
+      <c r="BB9" s="12"/>
+      <c r="BC9" s="12"/>
     </row>
     <row r="10" ht="56.05" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" t="s" s="11">
-        <v>181</v>
-      </c>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" t="s" s="11">
+      <c r="A10" s="10"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" t="s" s="13">
         <v>182</v>
       </c>
-      <c r="M10" s="10"/>
-      <c r="N10" t="s" s="11">
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" t="s" s="13">
         <v>183</v>
       </c>
-      <c r="O10" t="s" s="11">
+      <c r="M10" s="12"/>
+      <c r="N10" t="s" s="13">
         <v>184</v>
       </c>
-      <c r="P10" t="s" s="11">
+      <c r="O10" t="s" s="13">
         <v>185</v>
       </c>
-      <c r="Q10" t="s" s="11">
+      <c r="P10" t="s" s="13">
         <v>186</v>
       </c>
-      <c r="R10" t="s" s="11">
+      <c r="Q10" t="s" s="13">
         <v>187</v>
       </c>
-      <c r="S10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="U10" s="10"/>
-      <c r="V10" s="10"/>
-      <c r="W10" s="10"/>
-      <c r="X10" t="s" s="11">
+      <c r="R10" t="s" s="13">
         <v>188</v>
       </c>
-      <c r="Y10" t="s" s="11">
+      <c r="S10" s="12"/>
+      <c r="T10" s="12"/>
+      <c r="U10" s="12"/>
+      <c r="V10" s="12"/>
+      <c r="W10" s="12"/>
+      <c r="X10" t="s" s="13">
         <v>189</v>
       </c>
-      <c r="Z10" t="s" s="11">
+      <c r="Y10" t="s" s="13">
         <v>190</v>
       </c>
-      <c r="AA10" t="s" s="11">
+      <c r="Z10" t="s" s="13">
         <v>191</v>
       </c>
-      <c r="AB10" t="s" s="11">
+      <c r="AA10" t="s" s="13">
         <v>192</v>
       </c>
-      <c r="AC10" s="10"/>
-      <c r="AD10" t="s" s="11">
+      <c r="AB10" t="s" s="13">
         <v>193</v>
       </c>
-      <c r="AE10" s="10"/>
-      <c r="AF10" t="s" s="11">
+      <c r="AC10" s="12"/>
+      <c r="AD10" t="s" s="13">
         <v>194</v>
       </c>
-      <c r="AG10" s="10"/>
-      <c r="AH10" t="s" s="11">
+      <c r="AE10" s="12"/>
+      <c r="AF10" t="s" s="13">
         <v>195</v>
       </c>
-      <c r="AI10" s="10"/>
-      <c r="AJ10" t="s" s="11">
+      <c r="AG10" s="12"/>
+      <c r="AH10" t="s" s="13">
         <v>196</v>
       </c>
-      <c r="AK10" t="s" s="11">
+      <c r="AI10" s="12"/>
+      <c r="AJ10" t="s" s="13">
         <v>197</v>
       </c>
-      <c r="AL10" s="10"/>
-      <c r="AM10" s="10"/>
-      <c r="AN10" t="s" s="11">
+      <c r="AK10" t="s" s="13">
         <v>198</v>
       </c>
-      <c r="AO10" t="s" s="11">
+      <c r="AL10" s="12"/>
+      <c r="AM10" s="12"/>
+      <c r="AN10" t="s" s="13">
         <v>199</v>
       </c>
-      <c r="AP10" t="s" s="11">
+      <c r="AO10" t="s" s="13">
         <v>200</v>
       </c>
-      <c r="AQ10" s="10"/>
-      <c r="AR10" t="s" s="11">
+      <c r="AP10" t="s" s="13">
         <v>201</v>
       </c>
-      <c r="AS10" s="10"/>
-      <c r="AT10" t="s" s="11">
+      <c r="AQ10" s="12"/>
+      <c r="AR10" t="s" s="13">
         <v>202</v>
       </c>
-      <c r="AU10" t="s" s="11">
+      <c r="AS10" s="12"/>
+      <c r="AT10" t="s" s="13">
+        <v>203</v>
+      </c>
+      <c r="AU10" t="s" s="13">
         <v>97</v>
       </c>
-      <c r="AV10" t="s" s="11">
-        <v>203</v>
-      </c>
-      <c r="AW10" t="s" s="11">
+      <c r="AV10" t="s" s="13">
         <v>204</v>
       </c>
-      <c r="AX10" s="10"/>
-      <c r="AY10" s="10"/>
-      <c r="AZ10" s="10"/>
-      <c r="BA10" s="10"/>
-      <c r="BB10" s="10"/>
-      <c r="BC10" s="10"/>
+      <c r="AW10" t="s" s="13">
+        <v>205</v>
+      </c>
+      <c r="AX10" s="12"/>
+      <c r="AY10" s="12"/>
+      <c r="AZ10" s="12"/>
+      <c r="BA10" s="12"/>
+      <c r="BB10" s="12"/>
+      <c r="BC10" s="12"/>
     </row>
     <row r="11" ht="32.05" customHeight="1">
-      <c r="A11" s="8"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" t="s" s="11">
-        <v>205</v>
-      </c>
-      <c r="M11" t="s" s="11">
+      <c r="A11" s="10"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" t="s" s="13">
         <v>206</v>
       </c>
-      <c r="N11" t="s" s="11">
+      <c r="M11" t="s" s="13">
         <v>207</v>
       </c>
-      <c r="O11" s="10"/>
-      <c r="P11" t="s" s="11">
+      <c r="N11" t="s" s="13">
         <v>208</v>
       </c>
-      <c r="Q11" s="10"/>
-      <c r="R11" t="s" s="11">
+      <c r="O11" s="12"/>
+      <c r="P11" t="s" s="13">
         <v>209</v>
       </c>
-      <c r="S11" s="10"/>
-      <c r="T11" s="10"/>
-      <c r="U11" s="10"/>
-      <c r="V11" s="10"/>
-      <c r="W11" s="10"/>
-      <c r="X11" t="s" s="11">
+      <c r="Q11" s="12"/>
+      <c r="R11" t="s" s="13">
         <v>210</v>
       </c>
-      <c r="Y11" s="10"/>
-      <c r="Z11" t="s" s="11">
+      <c r="S11" s="12"/>
+      <c r="T11" s="12"/>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12"/>
+      <c r="X11" t="s" s="13">
         <v>211</v>
       </c>
-      <c r="AA11" t="s" s="11">
+      <c r="Y11" s="12"/>
+      <c r="Z11" t="s" s="13">
         <v>212</v>
       </c>
-      <c r="AB11" t="s" s="11">
+      <c r="AA11" t="s" s="13">
         <v>213</v>
       </c>
-      <c r="AC11" t="s" s="11">
+      <c r="AB11" t="s" s="13">
         <v>214</v>
       </c>
-      <c r="AD11" t="s" s="11">
+      <c r="AC11" s="13"/>
+      <c r="AD11" t="s" s="13">
         <v>215</v>
       </c>
-      <c r="AE11" s="10"/>
-      <c r="AF11" t="s" s="11">
+      <c r="AE11" s="12"/>
+      <c r="AF11" t="s" s="13">
         <v>216</v>
       </c>
-      <c r="AG11" t="s" s="11">
+      <c r="AG11" t="s" s="13">
         <v>217</v>
       </c>
-      <c r="AH11" s="10"/>
-      <c r="AI11" s="10"/>
-      <c r="AJ11" t="s" s="11">
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="12"/>
+      <c r="AJ11" t="s" s="13">
         <v>218</v>
       </c>
-      <c r="AK11" s="10"/>
-      <c r="AL11" s="10"/>
-      <c r="AM11" s="10"/>
-      <c r="AN11" t="s" s="11">
+      <c r="AK11" s="12"/>
+      <c r="AL11" s="12"/>
+      <c r="AM11" s="12"/>
+      <c r="AN11" t="s" s="13">
         <v>219</v>
       </c>
-      <c r="AO11" s="10"/>
-      <c r="AP11" s="10"/>
-      <c r="AQ11" s="10"/>
-      <c r="AR11" s="10"/>
-      <c r="AS11" s="10"/>
-      <c r="AT11" s="10"/>
-      <c r="AU11" s="10"/>
-      <c r="AV11" s="10"/>
-      <c r="AW11" s="10"/>
-      <c r="AX11" s="10"/>
-      <c r="AY11" s="10"/>
-      <c r="AZ11" s="10"/>
-      <c r="BA11" s="10"/>
-      <c r="BB11" s="10"/>
-      <c r="BC11" s="10"/>
+      <c r="AO11" s="12"/>
+      <c r="AP11" s="12"/>
+      <c r="AQ11" s="12"/>
+      <c r="AR11" s="12"/>
+      <c r="AS11" s="12"/>
+      <c r="AT11" s="12"/>
+      <c r="AU11" s="12"/>
+      <c r="AV11" s="12"/>
+      <c r="AW11" s="12"/>
+      <c r="AX11" s="12"/>
+      <c r="AY11" s="12"/>
+      <c r="AZ11" s="12"/>
+      <c r="BA11" s="12"/>
+      <c r="BB11" s="12"/>
+      <c r="BC11" s="12"/>
     </row>
     <row r="12" ht="44.05" customHeight="1">
-      <c r="A12" s="8"/>
-      <c r="B12" s="12"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" t="s" s="11">
+      <c r="A12" s="10"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="12"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="12"/>
+      <c r="L12" t="s" s="13">
         <v>220</v>
       </c>
-      <c r="M12" t="s" s="11">
+      <c r="M12" t="s" s="13">
         <v>221</v>
       </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" t="s" s="11">
+      <c r="N12" s="12"/>
+      <c r="O12" s="12"/>
+      <c r="P12" t="s" s="13">
         <v>222</v>
       </c>
-      <c r="Q12" t="s" s="11">
+      <c r="Q12" t="s" s="13">
         <v>223</v>
       </c>
-      <c r="R12" s="10"/>
-      <c r="S12" s="10"/>
-      <c r="T12" s="10"/>
-      <c r="U12" s="10"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" t="s" s="11">
+      <c r="R12" s="12"/>
+      <c r="S12" s="12"/>
+      <c r="T12" s="12"/>
+      <c r="U12" s="12"/>
+      <c r="V12" s="12"/>
+      <c r="W12" s="12"/>
+      <c r="X12" t="s" s="13">
         <v>224</v>
       </c>
-      <c r="Y12" s="10"/>
-      <c r="Z12" t="s" s="11">
+      <c r="Y12" s="12"/>
+      <c r="Z12" t="s" s="13">
         <v>225</v>
       </c>
-      <c r="AA12" s="10"/>
-      <c r="AB12" t="s" s="11">
+      <c r="AA12" s="12"/>
+      <c r="AB12" t="s" s="13">
         <v>226</v>
       </c>
-      <c r="AC12" s="10"/>
-      <c r="AD12" t="s" s="11">
+      <c r="AC12" s="12"/>
+      <c r="AD12" t="s" s="13">
         <v>227</v>
       </c>
-      <c r="AE12" s="10"/>
-      <c r="AF12" s="10"/>
-      <c r="AG12" s="10"/>
-      <c r="AH12" s="10"/>
-      <c r="AI12" s="10"/>
-      <c r="AJ12" t="s" s="11">
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AH12" s="12"/>
+      <c r="AI12" s="12"/>
+      <c r="AJ12" t="s" s="13">
         <v>228</v>
       </c>
-      <c r="AK12" s="10"/>
-      <c r="AL12" s="10"/>
-      <c r="AM12" s="10"/>
-      <c r="AN12" t="s" s="11">
+      <c r="AK12" s="12"/>
+      <c r="AL12" s="12"/>
+      <c r="AM12" s="12"/>
+      <c r="AN12" t="s" s="13">
         <v>229</v>
       </c>
-      <c r="AO12" s="10"/>
-      <c r="AP12" s="10"/>
-      <c r="AQ12" s="10"/>
-      <c r="AR12" s="10"/>
-      <c r="AS12" s="10"/>
-      <c r="AT12" s="10"/>
-      <c r="AU12" s="10"/>
-      <c r="AV12" s="10"/>
-      <c r="AW12" s="10"/>
-      <c r="AX12" s="10"/>
-      <c r="AY12" s="10"/>
-      <c r="AZ12" s="10"/>
-      <c r="BA12" s="10"/>
-      <c r="BB12" s="10"/>
-      <c r="BC12" s="10"/>
+      <c r="AO12" s="12"/>
+      <c r="AP12" s="12"/>
+      <c r="AQ12" s="12"/>
+      <c r="AR12" s="12"/>
+      <c r="AS12" s="12"/>
+      <c r="AT12" s="12"/>
+      <c r="AU12" s="12"/>
+      <c r="AV12" s="12"/>
+      <c r="AW12" s="12"/>
+      <c r="AX12" s="12"/>
+      <c r="AY12" s="12"/>
+      <c r="AZ12" s="12"/>
+      <c r="BA12" s="12"/>
+      <c r="BB12" s="12"/>
+      <c r="BC12" s="12"/>
     </row>
     <row r="13" ht="44.05" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="12"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
-      <c r="O13" s="10"/>
-      <c r="P13" s="10"/>
-      <c r="Q13" s="10"/>
-      <c r="R13" s="10"/>
-      <c r="S13" s="10"/>
-      <c r="T13" s="10"/>
-      <c r="U13" s="10"/>
-      <c r="V13" s="10"/>
-      <c r="W13" s="10"/>
-      <c r="X13" t="s" s="11">
+      <c r="A13" s="10"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="12"/>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12"/>
+      <c r="W13" s="12"/>
+      <c r="X13" t="s" s="13">
         <v>230</v>
       </c>
-      <c r="Y13" s="10"/>
-      <c r="Z13" t="s" s="11">
+      <c r="Y13" s="12"/>
+      <c r="Z13" t="s" s="13">
         <v>231</v>
       </c>
-      <c r="AA13" t="s" s="11">
+      <c r="AA13" t="s" s="13">
         <v>232</v>
       </c>
-      <c r="AB13" t="s" s="11">
+      <c r="AB13" t="s" s="13">
         <v>233</v>
       </c>
-      <c r="AC13" s="10"/>
-      <c r="AD13" t="s" s="11">
+      <c r="AC13" t="s" s="13">
         <v>234</v>
       </c>
-      <c r="AE13" s="10"/>
-      <c r="AF13" s="10"/>
-      <c r="AG13" s="10"/>
-      <c r="AH13" s="10"/>
-      <c r="AI13" s="10"/>
-      <c r="AJ13" s="10"/>
-      <c r="AK13" s="10"/>
-      <c r="AL13" s="10"/>
-      <c r="AM13" s="10"/>
-      <c r="AN13" t="s" s="11">
+      <c r="AD13" t="s" s="13">
         <v>235</v>
       </c>
-      <c r="AO13" t="s" s="11">
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
+      <c r="AG13" s="12"/>
+      <c r="AH13" s="12"/>
+      <c r="AI13" s="12"/>
+      <c r="AJ13" s="12"/>
+      <c r="AK13" s="12"/>
+      <c r="AL13" s="12"/>
+      <c r="AM13" s="12"/>
+      <c r="AN13" t="s" s="13">
         <v>236</v>
       </c>
-      <c r="AP13" s="10"/>
-      <c r="AQ13" s="10"/>
-      <c r="AR13" s="10"/>
-      <c r="AS13" s="10"/>
-      <c r="AT13" s="10"/>
-      <c r="AU13" s="10"/>
-      <c r="AV13" s="10"/>
-      <c r="AW13" s="10"/>
-      <c r="AX13" s="10"/>
-      <c r="AY13" s="10"/>
-      <c r="AZ13" s="10"/>
-      <c r="BA13" s="10"/>
-      <c r="BB13" s="10"/>
-      <c r="BC13" s="10"/>
+      <c r="AO13" t="s" s="13">
+        <v>237</v>
+      </c>
+      <c r="AP13" s="12"/>
+      <c r="AQ13" s="12"/>
+      <c r="AR13" s="12"/>
+      <c r="AS13" s="12"/>
+      <c r="AT13" s="12"/>
+      <c r="AU13" s="12"/>
+      <c r="AV13" s="12"/>
+      <c r="AW13" s="12"/>
+      <c r="AX13" s="12"/>
+      <c r="AY13" s="12"/>
+      <c r="AZ13" s="12"/>
+      <c r="BA13" s="12"/>
+      <c r="BB13" s="12"/>
+      <c r="BC13" s="12"/>
     </row>
     <row r="14" ht="32.05" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="12"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="10"/>
-      <c r="U14" s="10"/>
-      <c r="V14" s="10"/>
-      <c r="W14" s="10"/>
-      <c r="X14" s="10"/>
-      <c r="Y14" s="10"/>
-      <c r="Z14" t="s" s="11">
-        <v>237</v>
-      </c>
-      <c r="AA14" t="s" s="11">
+      <c r="A14" s="10"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="12"/>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="12"/>
+      <c r="U14" s="12"/>
+      <c r="V14" s="12"/>
+      <c r="W14" s="12"/>
+      <c r="X14" s="12"/>
+      <c r="Y14" s="12"/>
+      <c r="Z14" t="s" s="13">
         <v>238</v>
       </c>
-      <c r="AB14" t="s" s="11">
+      <c r="AA14" t="s" s="13">
         <v>239</v>
       </c>
-      <c r="AC14" s="10"/>
-      <c r="AD14" t="s" s="11">
+      <c r="AB14" t="s" s="13">
         <v>240</v>
       </c>
-      <c r="AE14" s="10"/>
-      <c r="AF14" s="10"/>
-      <c r="AG14" s="10"/>
-      <c r="AH14" s="10"/>
-      <c r="AI14" s="10"/>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="10"/>
-      <c r="AN14" s="10"/>
-      <c r="AO14" s="10"/>
-      <c r="AP14" s="10"/>
-      <c r="AQ14" s="10"/>
-      <c r="AR14" s="10"/>
-      <c r="AS14" s="10"/>
-      <c r="AT14" s="10"/>
-      <c r="AU14" s="10"/>
-      <c r="AV14" s="10"/>
-      <c r="AW14" s="10"/>
-      <c r="AX14" s="10"/>
-      <c r="AY14" s="10"/>
-      <c r="AZ14" s="10"/>
-      <c r="BA14" s="10"/>
-      <c r="BB14" s="10"/>
-      <c r="BC14" s="10"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" t="s" s="13">
+        <v>241</v>
+      </c>
+      <c r="AE14" s="12"/>
+      <c r="AF14" s="12"/>
+      <c r="AG14" s="12"/>
+      <c r="AH14" s="12"/>
+      <c r="AI14" s="12"/>
+      <c r="AJ14" s="12"/>
+      <c r="AK14" s="12"/>
+      <c r="AL14" s="12"/>
+      <c r="AM14" s="12"/>
+      <c r="AN14" s="12"/>
+      <c r="AO14" s="12"/>
+      <c r="AP14" s="12"/>
+      <c r="AQ14" s="12"/>
+      <c r="AR14" s="12"/>
+      <c r="AS14" s="12"/>
+      <c r="AT14" s="12"/>
+      <c r="AU14" s="12"/>
+      <c r="AV14" s="12"/>
+      <c r="AW14" s="12"/>
+      <c r="AX14" s="12"/>
+      <c r="AY14" s="12"/>
+      <c r="AZ14" s="12"/>
+      <c r="BA14" s="12"/>
+      <c r="BB14" s="12"/>
+      <c r="BC14" s="12"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="8"/>
-      <c r="B15" s="12"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="10"/>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="10"/>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="10"/>
-      <c r="U15" s="10"/>
-      <c r="V15" s="10"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="10"/>
-      <c r="Y15" s="10"/>
-      <c r="Z15" t="s" s="11">
-        <v>241</v>
-      </c>
-      <c r="AA15" s="10"/>
-      <c r="AB15" t="s" s="11">
+      <c r="A15" s="10"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="12"/>
+      <c r="M15" s="12"/>
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="12"/>
+      <c r="U15" s="12"/>
+      <c r="V15" s="12"/>
+      <c r="W15" s="12"/>
+      <c r="X15" s="12"/>
+      <c r="Y15" s="12"/>
+      <c r="Z15" t="s" s="13">
         <v>242</v>
       </c>
-      <c r="AC15" s="10"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="10"/>
-      <c r="AF15" s="10"/>
-      <c r="AG15" s="10"/>
-      <c r="AH15" s="10"/>
-      <c r="AI15" s="10"/>
-      <c r="AJ15" s="10"/>
-      <c r="AK15" s="10"/>
-      <c r="AL15" s="10"/>
-      <c r="AM15" s="10"/>
-      <c r="AN15" s="10"/>
-      <c r="AO15" s="10"/>
-      <c r="AP15" s="10"/>
-      <c r="AQ15" s="10"/>
-      <c r="AR15" s="10"/>
-      <c r="AS15" s="10"/>
-      <c r="AT15" s="10"/>
-      <c r="AU15" s="10"/>
-      <c r="AV15" s="10"/>
-      <c r="AW15" s="10"/>
-      <c r="AX15" s="10"/>
-      <c r="AY15" s="10"/>
-      <c r="AZ15" s="10"/>
-      <c r="BA15" s="10"/>
-      <c r="BB15" s="10"/>
-      <c r="BC15" s="10"/>
+      <c r="AA15" s="12"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="12"/>
+      <c r="AD15" s="12"/>
+      <c r="AE15" s="12"/>
+      <c r="AF15" s="12"/>
+      <c r="AG15" s="12"/>
+      <c r="AH15" s="12"/>
+      <c r="AI15" s="12"/>
+      <c r="AJ15" s="12"/>
+      <c r="AK15" s="12"/>
+      <c r="AL15" s="12"/>
+      <c r="AM15" s="12"/>
+      <c r="AN15" s="12"/>
+      <c r="AO15" s="12"/>
+      <c r="AP15" s="12"/>
+      <c r="AQ15" s="12"/>
+      <c r="AR15" s="12"/>
+      <c r="AS15" s="12"/>
+      <c r="AT15" s="12"/>
+      <c r="AU15" s="12"/>
+      <c r="AV15" s="12"/>
+      <c r="AW15" s="12"/>
+      <c r="AX15" s="12"/>
+      <c r="AY15" s="12"/>
+      <c r="AZ15" s="12"/>
+      <c r="BA15" s="12"/>
+      <c r="BB15" s="12"/>
+      <c r="BC15" s="12"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="8"/>
-      <c r="B16" s="12"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="10"/>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="10"/>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="10"/>
-      <c r="U16" s="10"/>
-      <c r="V16" s="10"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="10"/>
-      <c r="Y16" s="10"/>
-      <c r="Z16" s="10"/>
-      <c r="AA16" s="10"/>
-      <c r="AB16" s="10"/>
-      <c r="AC16" s="10"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="10"/>
-      <c r="AF16" s="10"/>
-      <c r="AG16" s="10"/>
-      <c r="AH16" s="10"/>
-      <c r="AI16" s="10"/>
-      <c r="AJ16" s="10"/>
-      <c r="AK16" s="10"/>
-      <c r="AL16" s="10"/>
-      <c r="AM16" s="10"/>
-      <c r="AN16" s="10"/>
-      <c r="AO16" s="10"/>
-      <c r="AP16" s="10"/>
-      <c r="AQ16" s="10"/>
-      <c r="AR16" s="10"/>
-      <c r="AS16" s="10"/>
-      <c r="AT16" s="10"/>
-      <c r="AU16" s="10"/>
-      <c r="AV16" s="10"/>
-      <c r="AW16" s="10"/>
-      <c r="AX16" s="10"/>
-      <c r="AY16" s="10"/>
-      <c r="AZ16" s="10"/>
-      <c r="BA16" s="10"/>
-      <c r="BB16" s="10"/>
-      <c r="BC16" s="10"/>
+      <c r="A16" s="10"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="12"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="12"/>
+      <c r="W16" s="12"/>
+      <c r="X16" s="12"/>
+      <c r="Y16" s="12"/>
+      <c r="Z16" s="12"/>
+      <c r="AA16" s="12"/>
+      <c r="AB16" s="12"/>
+      <c r="AC16" s="12"/>
+      <c r="AD16" s="12"/>
+      <c r="AE16" s="12"/>
+      <c r="AF16" s="12"/>
+      <c r="AG16" s="12"/>
+      <c r="AH16" s="12"/>
+      <c r="AI16" s="12"/>
+      <c r="AJ16" s="12"/>
+      <c r="AK16" s="12"/>
+      <c r="AL16" s="12"/>
+      <c r="AM16" s="12"/>
+      <c r="AN16" s="12"/>
+      <c r="AO16" s="12"/>
+      <c r="AP16" s="12"/>
+      <c r="AQ16" s="12"/>
+      <c r="AR16" s="12"/>
+      <c r="AS16" s="12"/>
+      <c r="AT16" s="12"/>
+      <c r="AU16" s="12"/>
+      <c r="AV16" s="12"/>
+      <c r="AW16" s="12"/>
+      <c r="AX16" s="12"/>
+      <c r="AY16" s="12"/>
+      <c r="AZ16" s="12"/>
+      <c r="BA16" s="12"/>
+      <c r="BB16" s="12"/>
+      <c r="BC16" s="12"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="8"/>
-      <c r="B17" s="12"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
-      <c r="T17" s="10"/>
-      <c r="U17" s="10"/>
-      <c r="V17" s="10"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="10"/>
-      <c r="Y17" s="10"/>
-      <c r="Z17" s="10"/>
-      <c r="AA17" s="10"/>
-      <c r="AB17" s="10"/>
-      <c r="AC17" s="10"/>
-      <c r="AD17" s="10"/>
-      <c r="AE17" s="10"/>
-      <c r="AF17" s="10"/>
-      <c r="AG17" s="10"/>
-      <c r="AH17" s="10"/>
-      <c r="AI17" s="10"/>
-      <c r="AJ17" s="10"/>
-      <c r="AK17" s="10"/>
-      <c r="AL17" s="10"/>
-      <c r="AM17" s="10"/>
-      <c r="AN17" s="10"/>
-      <c r="AO17" s="10"/>
-      <c r="AP17" s="10"/>
-      <c r="AQ17" s="10"/>
-      <c r="AR17" s="10"/>
-      <c r="AS17" s="10"/>
-      <c r="AT17" s="10"/>
-      <c r="AU17" s="10"/>
-      <c r="AV17" s="10"/>
-      <c r="AW17" s="10"/>
-      <c r="AX17" s="10"/>
-      <c r="AY17" s="10"/>
-      <c r="AZ17" s="10"/>
-      <c r="BA17" s="10"/>
-      <c r="BB17" s="10"/>
-      <c r="BC17" s="10"/>
+      <c r="A17" s="10"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="12"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="12"/>
+      <c r="U17" s="12"/>
+      <c r="V17" s="12"/>
+      <c r="W17" s="12"/>
+      <c r="X17" s="12"/>
+      <c r="Y17" s="12"/>
+      <c r="Z17" s="12"/>
+      <c r="AA17" s="12"/>
+      <c r="AB17" s="12"/>
+      <c r="AC17" s="12"/>
+      <c r="AD17" s="12"/>
+      <c r="AE17" s="12"/>
+      <c r="AF17" s="12"/>
+      <c r="AG17" s="12"/>
+      <c r="AH17" s="12"/>
+      <c r="AI17" s="12"/>
+      <c r="AJ17" s="12"/>
+      <c r="AK17" s="12"/>
+      <c r="AL17" s="12"/>
+      <c r="AM17" s="12"/>
+      <c r="AN17" s="12"/>
+      <c r="AO17" s="12"/>
+      <c r="AP17" s="12"/>
+      <c r="AQ17" s="12"/>
+      <c r="AR17" s="12"/>
+      <c r="AS17" s="12"/>
+      <c r="AT17" s="12"/>
+      <c r="AU17" s="12"/>
+      <c r="AV17" s="12"/>
+      <c r="AW17" s="12"/>
+      <c r="AX17" s="12"/>
+      <c r="AY17" s="12"/>
+      <c r="AZ17" s="12"/>
+      <c r="BA17" s="12"/>
+      <c r="BB17" s="12"/>
+      <c r="BC17" s="12"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="8"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
-      <c r="T18" s="10"/>
-      <c r="U18" s="10"/>
-      <c r="V18" s="10"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="10"/>
-      <c r="Y18" s="10"/>
-      <c r="Z18" s="10"/>
-      <c r="AA18" s="10"/>
-      <c r="AB18" s="10"/>
-      <c r="AC18" s="10"/>
-      <c r="AD18" s="10"/>
-      <c r="AE18" s="10"/>
-      <c r="AF18" s="10"/>
-      <c r="AG18" s="10"/>
-      <c r="AH18" s="10"/>
-      <c r="AI18" s="10"/>
-      <c r="AJ18" s="10"/>
-      <c r="AK18" s="10"/>
-      <c r="AL18" s="10"/>
-      <c r="AM18" s="10"/>
-      <c r="AN18" s="10"/>
-      <c r="AO18" s="10"/>
-      <c r="AP18" s="10"/>
-      <c r="AQ18" s="10"/>
-      <c r="AR18" s="10"/>
-      <c r="AS18" s="10"/>
-      <c r="AT18" s="10"/>
-      <c r="AU18" s="10"/>
-      <c r="AV18" s="10"/>
-      <c r="AW18" s="10"/>
-      <c r="AX18" s="10"/>
-      <c r="AY18" s="10"/>
-      <c r="AZ18" s="10"/>
-      <c r="BA18" s="10"/>
-      <c r="BB18" s="10"/>
-      <c r="BC18" s="10"/>
+      <c r="A18" s="10"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
+      <c r="AA18" s="12"/>
+      <c r="AB18" s="12"/>
+      <c r="AC18" s="12"/>
+      <c r="AD18" s="12"/>
+      <c r="AE18" s="12"/>
+      <c r="AF18" s="12"/>
+      <c r="AG18" s="12"/>
+      <c r="AH18" s="12"/>
+      <c r="AI18" s="12"/>
+      <c r="AJ18" s="12"/>
+      <c r="AK18" s="12"/>
+      <c r="AL18" s="12"/>
+      <c r="AM18" s="12"/>
+      <c r="AN18" s="12"/>
+      <c r="AO18" s="12"/>
+      <c r="AP18" s="12"/>
+      <c r="AQ18" s="12"/>
+      <c r="AR18" s="12"/>
+      <c r="AS18" s="12"/>
+      <c r="AT18" s="12"/>
+      <c r="AU18" s="12"/>
+      <c r="AV18" s="12"/>
+      <c r="AW18" s="12"/>
+      <c r="AX18" s="12"/>
+      <c r="AY18" s="12"/>
+      <c r="AZ18" s="12"/>
+      <c r="BA18" s="12"/>
+      <c r="BB18" s="12"/>
+      <c r="BC18" s="12"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="12"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="10"/>
-      <c r="L19" s="10"/>
-      <c r="M19" s="10"/>
-      <c r="N19" s="10"/>
-      <c r="O19" s="10"/>
-      <c r="P19" s="10"/>
-      <c r="Q19" s="10"/>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
-      <c r="T19" s="10"/>
-      <c r="U19" s="10"/>
-      <c r="V19" s="10"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="10"/>
-      <c r="Y19" s="10"/>
-      <c r="Z19" s="10"/>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="10"/>
-      <c r="AC19" s="10"/>
-      <c r="AD19" s="10"/>
-      <c r="AE19" s="10"/>
-      <c r="AF19" s="10"/>
-      <c r="AG19" s="10"/>
-      <c r="AH19" s="10"/>
-      <c r="AI19" s="10"/>
-      <c r="AJ19" s="10"/>
-      <c r="AK19" s="10"/>
-      <c r="AL19" s="10"/>
-      <c r="AM19" s="10"/>
-      <c r="AN19" s="10"/>
-      <c r="AO19" s="10"/>
-      <c r="AP19" s="10"/>
-      <c r="AQ19" s="10"/>
-      <c r="AR19" s="10"/>
-      <c r="AS19" s="10"/>
-      <c r="AT19" s="10"/>
-      <c r="AU19" s="10"/>
-      <c r="AV19" s="10"/>
-      <c r="AW19" s="10"/>
-      <c r="AX19" s="10"/>
-      <c r="AY19" s="10"/>
-      <c r="AZ19" s="10"/>
-      <c r="BA19" s="10"/>
-      <c r="BB19" s="10"/>
-      <c r="BC19" s="10"/>
+      <c r="A19" s="10"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="12"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="12"/>
+      <c r="N19" s="12"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="12"/>
+      <c r="Q19" s="12"/>
+      <c r="R19" s="12"/>
+      <c r="S19" s="12"/>
+      <c r="T19" s="12"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="12"/>
+      <c r="W19" s="12"/>
+      <c r="X19" s="12"/>
+      <c r="Y19" s="12"/>
+      <c r="Z19" s="12"/>
+      <c r="AA19" s="12"/>
+      <c r="AB19" s="12"/>
+      <c r="AC19" s="12"/>
+      <c r="AD19" s="12"/>
+      <c r="AE19" s="12"/>
+      <c r="AF19" s="12"/>
+      <c r="AG19" s="12"/>
+      <c r="AH19" s="12"/>
+      <c r="AI19" s="12"/>
+      <c r="AJ19" s="12"/>
+      <c r="AK19" s="12"/>
+      <c r="AL19" s="12"/>
+      <c r="AM19" s="12"/>
+      <c r="AN19" s="12"/>
+      <c r="AO19" s="12"/>
+      <c r="AP19" s="12"/>
+      <c r="AQ19" s="12"/>
+      <c r="AR19" s="12"/>
+      <c r="AS19" s="12"/>
+      <c r="AT19" s="12"/>
+      <c r="AU19" s="12"/>
+      <c r="AV19" s="12"/>
+      <c r="AW19" s="12"/>
+      <c r="AX19" s="12"/>
+      <c r="AY19" s="12"/>
+      <c r="AZ19" s="12"/>
+      <c r="BA19" s="12"/>
+      <c r="BB19" s="12"/>
+      <c r="BC19" s="12"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="12"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
-      <c r="O20" s="10"/>
-      <c r="P20" s="10"/>
-      <c r="Q20" s="10"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-      <c r="T20" s="10"/>
-      <c r="U20" s="10"/>
-      <c r="V20" s="10"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="10"/>
-      <c r="Y20" s="10"/>
-      <c r="Z20" s="10"/>
-      <c r="AA20" s="10"/>
-      <c r="AB20" s="10"/>
-      <c r="AC20" s="10"/>
-      <c r="AD20" s="10"/>
-      <c r="AE20" s="10"/>
-      <c r="AF20" s="10"/>
-      <c r="AG20" s="10"/>
-      <c r="AH20" s="10"/>
-      <c r="AI20" s="10"/>
-      <c r="AJ20" s="10"/>
-      <c r="AK20" s="10"/>
-      <c r="AL20" s="10"/>
-      <c r="AM20" s="10"/>
-      <c r="AN20" s="10"/>
-      <c r="AO20" s="10"/>
-      <c r="AP20" s="10"/>
-      <c r="AQ20" s="10"/>
-      <c r="AR20" s="10"/>
-      <c r="AS20" s="10"/>
-      <c r="AT20" s="10"/>
-      <c r="AU20" s="10"/>
-      <c r="AV20" s="10"/>
-      <c r="AW20" s="10"/>
-      <c r="AX20" s="10"/>
-      <c r="AY20" s="10"/>
-      <c r="AZ20" s="10"/>
-      <c r="BA20" s="10"/>
-      <c r="BB20" s="10"/>
-      <c r="BC20" s="10"/>
+      <c r="A20" s="10"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12"/>
+      <c r="M20" s="12"/>
+      <c r="N20" s="12"/>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="12"/>
+      <c r="S20" s="12"/>
+      <c r="T20" s="12"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12"/>
+      <c r="Y20" s="12"/>
+      <c r="Z20" s="12"/>
+      <c r="AA20" s="12"/>
+      <c r="AB20" s="12"/>
+      <c r="AC20" s="12"/>
+      <c r="AD20" s="12"/>
+      <c r="AE20" s="12"/>
+      <c r="AF20" s="12"/>
+      <c r="AG20" s="12"/>
+      <c r="AH20" s="12"/>
+      <c r="AI20" s="12"/>
+      <c r="AJ20" s="12"/>
+      <c r="AK20" s="12"/>
+      <c r="AL20" s="12"/>
+      <c r="AM20" s="12"/>
+      <c r="AN20" s="12"/>
+      <c r="AO20" s="12"/>
+      <c r="AP20" s="12"/>
+      <c r="AQ20" s="12"/>
+      <c r="AR20" s="12"/>
+      <c r="AS20" s="12"/>
+      <c r="AT20" s="12"/>
+      <c r="AU20" s="12"/>
+      <c r="AV20" s="12"/>
+      <c r="AW20" s="12"/>
+      <c r="AX20" s="12"/>
+      <c r="AY20" s="12"/>
+      <c r="AZ20" s="12"/>
+      <c r="BA20" s="12"/>
+      <c r="BB20" s="12"/>
+      <c r="BC20" s="12"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="12"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="10"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
-      <c r="T21" s="10"/>
-      <c r="U21" s="10"/>
-      <c r="V21" s="10"/>
-      <c r="W21" s="10"/>
-      <c r="X21" s="10"/>
-      <c r="Y21" s="10"/>
-      <c r="Z21" s="10"/>
-      <c r="AA21" s="10"/>
-      <c r="AB21" s="10"/>
-      <c r="AC21" s="10"/>
-      <c r="AD21" s="10"/>
-      <c r="AE21" s="10"/>
-      <c r="AF21" s="10"/>
-      <c r="AG21" s="10"/>
-      <c r="AH21" s="10"/>
-      <c r="AI21" s="10"/>
-      <c r="AJ21" s="10"/>
-      <c r="AK21" s="10"/>
-      <c r="AL21" s="10"/>
-      <c r="AM21" s="10"/>
-      <c r="AN21" s="10"/>
-      <c r="AO21" s="10"/>
-      <c r="AP21" s="10"/>
-      <c r="AQ21" s="10"/>
-      <c r="AR21" s="10"/>
-      <c r="AS21" s="10"/>
-      <c r="AT21" s="10"/>
-      <c r="AU21" s="10"/>
-      <c r="AV21" s="10"/>
-      <c r="AW21" s="10"/>
-      <c r="AX21" s="10"/>
-      <c r="AY21" s="10"/>
-      <c r="AZ21" s="10"/>
-      <c r="BA21" s="10"/>
-      <c r="BB21" s="10"/>
-      <c r="BC21" s="10"/>
+      <c r="A21" s="10"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="12"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="12"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="12"/>
+      <c r="N21" s="12"/>
+      <c r="O21" s="12"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="12"/>
+      <c r="S21" s="12"/>
+      <c r="T21" s="12"/>
+      <c r="U21" s="12"/>
+      <c r="V21" s="12"/>
+      <c r="W21" s="12"/>
+      <c r="X21" s="12"/>
+      <c r="Y21" s="12"/>
+      <c r="Z21" s="12"/>
+      <c r="AA21" s="12"/>
+      <c r="AB21" s="12"/>
+      <c r="AC21" s="12"/>
+      <c r="AD21" s="12"/>
+      <c r="AE21" s="12"/>
+      <c r="AF21" s="12"/>
+      <c r="AG21" s="12"/>
+      <c r="AH21" s="12"/>
+      <c r="AI21" s="12"/>
+      <c r="AJ21" s="12"/>
+      <c r="AK21" s="12"/>
+      <c r="AL21" s="12"/>
+      <c r="AM21" s="12"/>
+      <c r="AN21" s="12"/>
+      <c r="AO21" s="12"/>
+      <c r="AP21" s="12"/>
+      <c r="AQ21" s="12"/>
+      <c r="AR21" s="12"/>
+      <c r="AS21" s="12"/>
+      <c r="AT21" s="12"/>
+      <c r="AU21" s="12"/>
+      <c r="AV21" s="12"/>
+      <c r="AW21" s="12"/>
+      <c r="AX21" s="12"/>
+      <c r="AY21" s="12"/>
+      <c r="AZ21" s="12"/>
+      <c r="BA21" s="12"/>
+      <c r="BB21" s="12"/>
+      <c r="BC21" s="12"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="12"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
-      <c r="T22" s="10"/>
-      <c r="U22" s="10"/>
-      <c r="V22" s="10"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="10"/>
-      <c r="Y22" s="10"/>
-      <c r="Z22" s="10"/>
-      <c r="AA22" s="10"/>
-      <c r="AB22" s="10"/>
-      <c r="AC22" s="10"/>
-      <c r="AD22" s="10"/>
-      <c r="AE22" s="10"/>
-      <c r="AF22" s="10"/>
-      <c r="AG22" s="10"/>
-      <c r="AH22" s="10"/>
-      <c r="AI22" s="10"/>
-      <c r="AJ22" s="10"/>
-      <c r="AK22" s="10"/>
-      <c r="AL22" s="10"/>
-      <c r="AM22" s="10"/>
-      <c r="AN22" s="10"/>
-      <c r="AO22" s="10"/>
-      <c r="AP22" s="10"/>
-      <c r="AQ22" s="10"/>
-      <c r="AR22" s="10"/>
-      <c r="AS22" s="10"/>
-      <c r="AT22" s="10"/>
-      <c r="AU22" s="10"/>
-      <c r="AV22" s="10"/>
-      <c r="AW22" s="10"/>
-      <c r="AX22" s="10"/>
-      <c r="AY22" s="10"/>
-      <c r="AZ22" s="10"/>
-      <c r="BA22" s="10"/>
-      <c r="BB22" s="10"/>
-      <c r="BC22" s="10"/>
+      <c r="A22" s="10"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="12"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="12"/>
+      <c r="N22" s="12"/>
+      <c r="O22" s="12"/>
+      <c r="P22" s="12"/>
+      <c r="Q22" s="12"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="12"/>
+      <c r="T22" s="12"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="12"/>
+      <c r="W22" s="12"/>
+      <c r="X22" s="12"/>
+      <c r="Y22" s="12"/>
+      <c r="Z22" s="12"/>
+      <c r="AA22" s="12"/>
+      <c r="AB22" s="12"/>
+      <c r="AC22" s="12"/>
+      <c r="AD22" s="12"/>
+      <c r="AE22" s="12"/>
+      <c r="AF22" s="12"/>
+      <c r="AG22" s="12"/>
+      <c r="AH22" s="12"/>
+      <c r="AI22" s="12"/>
+      <c r="AJ22" s="12"/>
+      <c r="AK22" s="12"/>
+      <c r="AL22" s="12"/>
+      <c r="AM22" s="12"/>
+      <c r="AN22" s="12"/>
+      <c r="AO22" s="12"/>
+      <c r="AP22" s="12"/>
+      <c r="AQ22" s="12"/>
+      <c r="AR22" s="12"/>
+      <c r="AS22" s="12"/>
+      <c r="AT22" s="12"/>
+      <c r="AU22" s="12"/>
+      <c r="AV22" s="12"/>
+      <c r="AW22" s="12"/>
+      <c r="AX22" s="12"/>
+      <c r="AY22" s="12"/>
+      <c r="AZ22" s="12"/>
+      <c r="BA22" s="12"/>
+      <c r="BB22" s="12"/>
+      <c r="BC22" s="12"/>
     </row>
     <row r="23" ht="20.05" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="12"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
-      <c r="T23" s="10"/>
-      <c r="U23" s="10"/>
-      <c r="V23" s="10"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="10"/>
-      <c r="Y23" s="10"/>
-      <c r="Z23" s="10"/>
-      <c r="AA23" s="10"/>
-      <c r="AB23" s="10"/>
-      <c r="AC23" s="10"/>
-      <c r="AD23" s="10"/>
-      <c r="AE23" s="10"/>
-      <c r="AF23" s="10"/>
-      <c r="AG23" s="10"/>
-      <c r="AH23" s="10"/>
-      <c r="AI23" s="10"/>
-      <c r="AJ23" s="10"/>
-      <c r="AK23" s="10"/>
-      <c r="AL23" s="10"/>
-      <c r="AM23" s="10"/>
-      <c r="AN23" s="10"/>
-      <c r="AO23" s="10"/>
-      <c r="AP23" s="10"/>
-      <c r="AQ23" s="10"/>
-      <c r="AR23" s="10"/>
-      <c r="AS23" s="10"/>
-      <c r="AT23" s="10"/>
-      <c r="AU23" s="10"/>
-      <c r="AV23" s="10"/>
-      <c r="AW23" s="10"/>
-      <c r="AX23" s="10"/>
-      <c r="AY23" s="10"/>
-      <c r="AZ23" s="10"/>
-      <c r="BA23" s="10"/>
-      <c r="BB23" s="10"/>
-      <c r="BC23" s="10"/>
+      <c r="A23" s="10"/>
+      <c r="B23" s="14"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12"/>
+      <c r="Z23" s="12"/>
+      <c r="AA23" s="12"/>
+      <c r="AB23" s="12"/>
+      <c r="AC23" s="12"/>
+      <c r="AD23" s="12"/>
+      <c r="AE23" s="12"/>
+      <c r="AF23" s="12"/>
+      <c r="AG23" s="12"/>
+      <c r="AH23" s="12"/>
+      <c r="AI23" s="12"/>
+      <c r="AJ23" s="12"/>
+      <c r="AK23" s="12"/>
+      <c r="AL23" s="12"/>
+      <c r="AM23" s="12"/>
+      <c r="AN23" s="12"/>
+      <c r="AO23" s="12"/>
+      <c r="AP23" s="12"/>
+      <c r="AQ23" s="12"/>
+      <c r="AR23" s="12"/>
+      <c r="AS23" s="12"/>
+      <c r="AT23" s="12"/>
+      <c r="AU23" s="12"/>
+      <c r="AV23" s="12"/>
+      <c r="AW23" s="12"/>
+      <c r="AX23" s="12"/>
+      <c r="AY23" s="12"/>
+      <c r="AZ23" s="12"/>
+      <c r="BA23" s="12"/>
+      <c r="BB23" s="12"/>
+      <c r="BC23" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>